<commit_message>
add checklist data update
</commit_message>
<xml_diff>
--- a/datasets/rl-libellen-checklist/data/raw/Odonata_Checklist.xlsx
+++ b/datasets/rl-libellen-checklist/data/raw/Odonata_Checklist.xlsx
@@ -10,12 +10,15 @@
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
     <sheet name="Rode Lijst 2021" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Checklist!$A$1:$D$73</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="164">
   <si>
     <t>sort_id</t>
   </si>
@@ -446,24 +449,15 @@
     <t>Sympetrum vulgatum (Linnaeus, 1758)</t>
   </si>
   <si>
-    <t>71*</t>
-  </si>
-  <si>
     <t>Senegalees lantaarntje</t>
   </si>
   <si>
     <t>Ischnura senegalensis (Rambur, 1842)</t>
   </si>
   <si>
-    <t>72*</t>
-  </si>
-  <si>
     <t>Pseudagrion microcephalum (Rambur, 1842)</t>
   </si>
   <si>
-    <t>* = exotic species/non native</t>
-  </si>
-  <si>
     <t>Ned Naam</t>
   </si>
   <si>
@@ -501,6 +495,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>non native</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
+    <t>establishmentMeans</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>Animalia</t>
   </si>
 </sst>
 </file>
@@ -963,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,9 +983,10 @@
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -986,8 +996,14 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -997,8 +1013,14 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1008,8 +1030,14 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1019,8 +1047,14 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1030,8 +1064,14 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1041,8 +1081,14 @@
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1052,8 +1098,14 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1063,8 +1115,14 @@
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1074,8 +1132,14 @@
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1085,8 +1149,14 @@
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1096,8 +1166,14 @@
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1107,8 +1183,14 @@
       <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1118,8 +1200,14 @@
       <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1129,8 +1217,14 @@
       <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1140,8 +1234,14 @@
       <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1151,8 +1251,14 @@
       <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1162,8 +1268,14 @@
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1173,8 +1285,14 @@
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1184,8 +1302,14 @@
       <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1195,8 +1319,14 @@
       <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1206,8 +1336,14 @@
       <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1217,8 +1353,14 @@
       <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1228,8 +1370,14 @@
       <c r="C23" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1239,8 +1387,14 @@
       <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1250,8 +1404,14 @@
       <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1261,8 +1421,14 @@
       <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1272,8 +1438,14 @@
       <c r="C27" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1283,8 +1455,14 @@
       <c r="C28" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1294,8 +1472,14 @@
       <c r="C29" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1305,8 +1489,14 @@
       <c r="C30" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1316,8 +1506,14 @@
       <c r="C31" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1327,8 +1523,14 @@
       <c r="C32" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1338,8 +1540,14 @@
       <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1349,8 +1557,14 @@
       <c r="C34" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1360,8 +1574,14 @@
       <c r="C35" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1371,8 +1591,14 @@
       <c r="C36" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1382,8 +1608,14 @@
       <c r="C37" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1393,8 +1625,14 @@
       <c r="C38" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1404,8 +1642,14 @@
       <c r="C39" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1415,8 +1659,14 @@
       <c r="C40" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1426,8 +1676,14 @@
       <c r="C41" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>160</v>
+      </c>
+      <c r="E41" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1437,8 +1693,14 @@
       <c r="C42" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1448,8 +1710,14 @@
       <c r="C43" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1459,8 +1727,14 @@
       <c r="C44" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1470,8 +1744,14 @@
       <c r="C45" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>160</v>
+      </c>
+      <c r="E45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1481,8 +1761,14 @@
       <c r="C46" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1492,8 +1778,14 @@
       <c r="C47" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1503,8 +1795,14 @@
       <c r="C48" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1514,8 +1812,14 @@
       <c r="C49" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>160</v>
+      </c>
+      <c r="E49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1525,8 +1829,14 @@
       <c r="C50" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1536,8 +1846,14 @@
       <c r="C51" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>160</v>
+      </c>
+      <c r="E51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1547,8 +1863,14 @@
       <c r="C52" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>160</v>
+      </c>
+      <c r="E52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1558,8 +1880,14 @@
       <c r="C53" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1569,8 +1897,14 @@
       <c r="C54" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>160</v>
+      </c>
+      <c r="E54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1580,8 +1914,14 @@
       <c r="C55" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1591,8 +1931,14 @@
       <c r="C56" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1602,8 +1948,14 @@
       <c r="C57" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1613,8 +1965,14 @@
       <c r="C58" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1624,8 +1982,14 @@
       <c r="C59" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>160</v>
+      </c>
+      <c r="E59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1635,8 +1999,14 @@
       <c r="C60" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>160</v>
+      </c>
+      <c r="E60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1646,8 +2016,14 @@
       <c r="C61" s="3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>160</v>
+      </c>
+      <c r="E61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1657,8 +2033,14 @@
       <c r="C62" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>160</v>
+      </c>
+      <c r="E62" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1668,8 +2050,14 @@
       <c r="C63" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>160</v>
+      </c>
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1679,8 +2067,14 @@
       <c r="C64" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1690,8 +2084,14 @@
       <c r="C65" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>160</v>
+      </c>
+      <c r="E65" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1701,8 +2101,14 @@
       <c r="C66" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>160</v>
+      </c>
+      <c r="E66" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1712,8 +2118,14 @@
       <c r="C67" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>160</v>
+      </c>
+      <c r="E67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1723,8 +2135,14 @@
       <c r="C68" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>160</v>
+      </c>
+      <c r="E68" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1734,8 +2152,14 @@
       <c r="C69" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>160</v>
+      </c>
+      <c r="E69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1745,8 +2169,14 @@
       <c r="C70" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>160</v>
+      </c>
+      <c r="E70" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1756,29 +2186,42 @@
       <c r="C71" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="D71" t="s">
+        <v>160</v>
+      </c>
+      <c r="E71" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>144</v>
+      </c>
+      <c r="D72" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>146</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>148</v>
+      <c r="D73" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1807,13 +2250,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1827,7 +2270,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1841,7 +2284,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1855,7 +2298,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1863,13 +2306,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1883,7 +2326,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1897,7 +2340,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1911,7 +2354,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1925,7 +2368,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E9" s="15"/>
     </row>
@@ -1940,7 +2383,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1954,7 +2397,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1968,7 +2411,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1982,7 +2425,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1996,7 +2439,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2010,7 +2453,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2024,7 +2467,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2038,7 +2481,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2052,7 +2495,7 @@
         <v>36</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2066,7 +2509,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2080,7 +2523,7 @@
         <v>40</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2094,7 +2537,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2108,7 +2551,7 @@
         <v>44</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,7 +2565,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2136,7 +2579,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2150,7 +2593,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2164,7 +2607,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2178,7 +2621,7 @@
         <v>54</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2192,7 +2635,7 @@
         <v>56</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2206,7 +2649,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2220,7 +2663,7 @@
         <v>60</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2234,7 +2677,7 @@
         <v>62</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2248,7 +2691,7 @@
         <v>64</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2262,7 +2705,7 @@
         <v>66</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2276,7 +2719,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2290,7 +2733,7 @@
         <v>70</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2304,7 +2747,7 @@
         <v>72</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2318,7 +2761,7 @@
         <v>74</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2332,7 +2775,7 @@
         <v>76</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2346,7 +2789,7 @@
         <v>78</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2360,7 +2803,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2374,7 +2817,7 @@
         <v>82</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2388,7 +2831,7 @@
         <v>84</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2402,7 +2845,7 @@
         <v>86</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2416,7 +2859,7 @@
         <v>88</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2430,7 +2873,7 @@
         <v>90</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2444,7 +2887,7 @@
         <v>92</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2458,7 +2901,7 @@
         <v>94</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2472,7 +2915,7 @@
         <v>96</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2486,7 +2929,7 @@
         <v>98</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2500,7 +2943,7 @@
         <v>100</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2514,7 +2957,7 @@
         <v>102</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2528,7 +2971,7 @@
         <v>104</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2542,7 +2985,7 @@
         <v>106</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2556,7 +2999,7 @@
         <v>108</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2570,7 +3013,7 @@
         <v>110</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2584,7 +3027,7 @@
         <v>112</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2598,7 +3041,7 @@
         <v>114</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2612,7 +3055,7 @@
         <v>116</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2626,7 +3069,7 @@
         <v>118</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2640,7 +3083,7 @@
         <v>120</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2654,7 +3097,7 @@
         <v>122</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2668,7 +3111,7 @@
         <v>124</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2682,7 +3125,7 @@
         <v>126</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2696,7 +3139,7 @@
         <v>128</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2710,7 +3153,7 @@
         <v>130</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2724,7 +3167,7 @@
         <v>132</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2738,7 +3181,7 @@
         <v>134</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2752,7 +3195,7 @@
         <v>136</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2766,7 +3209,7 @@
         <v>138</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2780,7 +3223,7 @@
         <v>140</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2794,7 +3237,7 @@
         <v>142</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2802,7 +3245,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>